<commit_message>
final optimization from template
</commit_message>
<xml_diff>
--- a/testData/test_data.xlsx
+++ b/testData/test_data.xlsx
@@ -8,20 +8,34 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rfnsh\PycharmProjects\Web-Automation-With-Python\testData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1322BAD3-E7AC-40A1-B778-1524A3D75EA8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{116620C8-57D5-4213-8641-354351D1CE3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="configuration" sheetId="1" r:id="rId1"/>
     <sheet name="login" sheetId="2" r:id="rId2"/>
+    <sheet name="urls" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="28">
   <si>
     <t>api_url</t>
   </si>
@@ -87,6 +101,24 @@
   </si>
   <si>
     <t>https://api.rahulshettyacademy.com/angularpractice/</t>
+  </si>
+  <si>
+    <t>stage</t>
+  </si>
+  <si>
+    <t>qa</t>
+  </si>
+  <si>
+    <t>dev</t>
+  </si>
+  <si>
+    <t>prod</t>
+  </si>
+  <si>
+    <t>https://dev.rahulshettyacademy.com/angularpractice/</t>
+  </si>
+  <si>
+    <t>https://prod.rahulshettyacademy.com/angularpractice/</t>
   </si>
 </sst>
 </file>
@@ -477,93 +509,112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" customWidth="1"/>
-    <col min="2" max="2" width="34.109375" customWidth="1"/>
-    <col min="3" max="3" width="45.6640625" customWidth="1"/>
-    <col min="4" max="4" width="15.88671875" customWidth="1"/>
-    <col min="5" max="5" width="12.88671875" customWidth="1"/>
-    <col min="6" max="6" width="17.109375" customWidth="1"/>
-    <col min="7" max="7" width="25.44140625" customWidth="1"/>
-    <col min="8" max="8" width="24.5546875" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="48.140625" customWidth="1"/>
+    <col min="4" max="4" width="49.140625" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" customWidth="1"/>
+    <col min="6" max="6" width="12.85546875" customWidth="1"/>
+    <col min="7" max="7" width="17.140625" customWidth="1"/>
+    <col min="8" max="8" width="25.42578125" customWidth="1"/>
+    <col min="9" max="9" width="24.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="7" t="s">
         <v>14</v>
       </c>
-      <c r="B1" s="4" t="s">
+      <c r="C1" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="D1" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="4" t="s">
+      <c r="H1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="4" t="s">
+      <c r="I1" s="4" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="30" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:9" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="C2" s="8" t="s">
         <v>21</v>
       </c>
-      <c r="C2" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="D2" s="3" t="s">
+      <c r="D2" s="6" t="str">
+        <f>VLOOKUP(A2,urls!A1:B3,2,FALSE)</f>
+        <v>https://rahulshettyacademy.com/angularpractice/</v>
+      </c>
+      <c r="E2" s="3" t="s">
         <v>16</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>6</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>15</v>
       </c>
       <c r="G2" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>17</v>
       </c>
     </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="G2" xr:uid="{00000000-0002-0000-0000-000000000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="H2" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"UI, API, Both"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E2:F2" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="F2:G2" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"no, yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="D2" xr:uid="{00000000-0002-0000-0000-000002000000}">
+    <dataValidation type="list" showInputMessage="1" showErrorMessage="1" sqref="E2" xr:uid="{00000000-0002-0000-0000-000002000000}">
       <formula1>"Chrome, Firefox, Edge, Opera"</formula1>
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" xr:uid="{8CCC3C5E-2CE0-4627-8224-3848495678BB}"/>
+    <hyperlink ref="C2" r:id="rId1" xr:uid="{8CCC3C5E-2CE0-4627-8224-3848495678BB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
+        <x14:dataValidation type="list" showInputMessage="1" showErrorMessage="1" xr:uid="{E1566892-E3D6-4CBD-9483-17366AB17204}">
+          <x14:formula1>
+            <xm:f>urls!$A$1:$A$3</xm:f>
+          </x14:formula1>
+          <xm:sqref>A2</xm:sqref>
+        </x14:dataValidation>
+      </x14:dataValidations>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -575,15 +626,15 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18.109375" customWidth="1"/>
-    <col min="2" max="2" width="33.109375" customWidth="1"/>
+    <col min="1" max="1" width="18.140625" customWidth="1"/>
+    <col min="2" max="2" width="33.140625" customWidth="1"/>
     <col min="3" max="3" width="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
         <v>7</v>
       </c>
@@ -591,7 +642,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
         <v>9</v>
       </c>
@@ -602,7 +653,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="B8" s="2" t="s">
         <v>7</v>
       </c>
@@ -610,7 +661,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
         <v>12</v>
       </c>
@@ -630,4 +681,51 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{16A6CC52-174A-4396-96A9-E182E804654A}">
+  <dimension ref="A1:B3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="46.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B1" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="8" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" s="8" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B1" r:id="rId1" xr:uid="{61F225A1-7A89-4AFF-89D7-1DD5E80A2DC2}"/>
+    <hyperlink ref="B2" r:id="rId2" xr:uid="{038D00E3-CC8B-4662-940A-E47280E10213}"/>
+    <hyperlink ref="B3" r:id="rId3" xr:uid="{851D8AD6-6E7E-4BB3-9533-E7A1BD33EAD9}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>